<commit_message>
AO-ET: Fixed regex issues.
</commit_message>
<xml_diff>
--- a/SCH-STH/Baseline Mapping/Angola/May 2021/ao_sch_sth_baseline_4_urinefiltration_202105.xlsx
+++ b/SCH-STH/Baseline Mapping/Angola/May 2021/ao_sch_sth_baseline_4_urinefiltration_202105.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\SCH-STH\Baseline Mapping\Angola\May 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231AADE2-E508-48EA-ACF2-BAFEC6D9C399}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33A5D2A-7CAC-4386-837E-74BD23F98520}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1946,9 +1946,6 @@
     <t>Escola Primaria Nº 36 De Santa</t>
   </si>
   <si>
-    <t>regex(.,'^[0-9]{3}-[0-9]{6}-[0-3]{3}$')</t>
-  </si>
-  <si>
     <t>Insira ID exclusivo a partir do teste de diagnóstico (deve ser insierido como 123-123456-123 letras maiúsculas com traços)</t>
   </si>
   <si>
@@ -1968,6 +1965,9 @@
   </si>
   <si>
     <t>4. Resultados do formulário - Urine Filtration CCA</t>
+  </si>
+  <si>
+    <t>regex(.,'^[0-9]{3}-[0-9]{6}-[0-9]{3}$')</t>
   </si>
 </sst>
 </file>
@@ -2485,10 +2485,10 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2784,29 +2784,29 @@
         <v>91</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="11" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="12" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="13"/>
       <c r="J8" s="24" t="s">
-        <v>638</v>
+        <v>645</v>
       </c>
       <c r="K8" s="8" t="s">
+        <v>641</v>
+      </c>
+      <c r="L8" s="11" t="s">
         <v>642</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="M8" s="12" t="s">
         <v>643</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>644</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="13"/>
@@ -20882,7 +20882,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B2" t="s">
         <v>102</v>

</xml_diff>